<commit_message>
testing some other stuff for LOI and trap GSD
</commit_message>
<xml_diff>
--- a/GSD/baskets_new_sizes/basketGSD_hypflux_NEW_SIZES (version 1) (version 1).xlsb.xlsx
+++ b/GSD/baskets_new_sizes/basketGSD_hypflux_NEW_SIZES (version 1) (version 1).xlsb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\GSD\baskets_new_sizes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\baskets_new_sizes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E165E88-C349-4E0B-A076-2176B018B6B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F256F24-2206-4C69-AB45-E09455A8D5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FF2C68C4-0230-4397-BD30-01ABAA0FCBBF}"/>
+    <workbookView minimized="1" xWindow="3120" yWindow="660" windowWidth="22260" windowHeight="14940" xr2:uid="{FF2C68C4-0230-4397-BD30-01ABAA0FCBBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Spring Weights" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Regression" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2603,125 +2602,125 @@
     <xf numFmtId="165" fontId="3" fillId="21" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2848,7 +2847,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2936,7 +2935,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-AR"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3116,7 +3115,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-AR"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3302,7 +3301,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-AR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3340,7 +3339,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="795026224"/>
@@ -3426,7 +3425,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-AR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3464,7 +3463,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="795026704"/>
@@ -3514,7 +3513,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3551,7 +3550,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3634,7 +3633,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3722,7 +3721,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-AR"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3896,7 +3895,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-AR"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4082,7 +4081,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-AR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4120,7 +4119,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="795026224"/>
@@ -4206,7 +4205,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-AR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4244,7 +4243,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="795026704"/>
@@ -4294,7 +4293,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4331,7 +4330,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4415,7 +4414,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4511,7 +4510,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-AR"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4693,7 +4692,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-AR"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4875,7 +4874,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-AR"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -5057,7 +5056,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-AR"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -5236,7 +5235,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-AR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5274,7 +5273,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1581415840"/>
@@ -5372,7 +5371,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-AR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5410,7 +5409,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1581418720"/>
@@ -5468,7 +5467,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5505,7 +5504,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5589,7 +5588,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5685,7 +5684,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-AR"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -5861,7 +5860,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-AR"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -6037,7 +6036,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-AR"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -6213,7 +6212,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-AR"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -6386,7 +6385,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-AR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6424,7 +6423,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1581415840"/>
@@ -6522,7 +6521,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-AR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6560,7 +6559,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1581418720"/>
@@ -6618,7 +6617,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6655,7 +6654,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9376,45 +9375,45 @@
       <selection activeCell="AM6" sqref="AM6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.75" customWidth="1"/>
     <col min="27" max="27" width="18" customWidth="1"/>
-    <col min="28" max="28" width="22.44140625" customWidth="1"/>
+    <col min="28" max="28" width="22.5" customWidth="1"/>
     <col min="29" max="29" width="19" customWidth="1"/>
-    <col min="30" max="30" width="18.6640625" customWidth="1"/>
-    <col min="31" max="31" width="16.77734375" customWidth="1"/>
-    <col min="32" max="32" width="19.109375" customWidth="1"/>
-    <col min="33" max="33" width="20.88671875" customWidth="1"/>
-    <col min="34" max="34" width="17.33203125" customWidth="1"/>
-    <col min="35" max="35" width="20.21875" customWidth="1"/>
-    <col min="36" max="36" width="18.21875" customWidth="1"/>
+    <col min="30" max="30" width="18.625" customWidth="1"/>
+    <col min="31" max="31" width="16.75" customWidth="1"/>
+    <col min="32" max="32" width="19.125" customWidth="1"/>
+    <col min="33" max="33" width="20.875" customWidth="1"/>
+    <col min="34" max="34" width="17.375" customWidth="1"/>
+    <col min="35" max="35" width="20.25" customWidth="1"/>
+    <col min="36" max="36" width="18.25" customWidth="1"/>
     <col min="37" max="37" width="17" customWidth="1"/>
-    <col min="38" max="38" width="14.5546875" customWidth="1"/>
-    <col min="39" max="39" width="14.6640625" customWidth="1"/>
+    <col min="38" max="38" width="14.5" customWidth="1"/>
+    <col min="39" max="39" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AG1" s="476" t="s">
+    <row r="1" spans="2:38" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG1" s="458" t="s">
         <v>56</v>
       </c>
-      <c r="AH1" s="476" t="s">
+      <c r="AH1" s="458" t="s">
         <v>57</v>
       </c>
-      <c r="AI1" s="476" t="s">
+      <c r="AI1" s="458" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="476" t="s">
+      <c r="AJ1" s="458" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="485" t="s">
+      <c r="AK1" s="452" t="s">
         <v>57</v>
       </c>
-      <c r="AL1" s="485" t="s">
+      <c r="AL1" s="452" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="2:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -9487,25 +9486,25 @@
       <c r="Y2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AB2" s="488" t="s">
+      <c r="AB2" s="455" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="489"/>
-      <c r="AD2" s="483" t="s">
+      <c r="AC2" s="456"/>
+      <c r="AD2" s="459" t="s">
         <v>58</v>
       </c>
-      <c r="AE2" s="483"/>
+      <c r="AE2" s="459"/>
       <c r="AF2" s="102" t="s">
         <v>105</v>
       </c>
-      <c r="AG2" s="491"/>
-      <c r="AH2" s="476"/>
-      <c r="AI2" s="476"/>
-      <c r="AJ2" s="476"/>
-      <c r="AK2" s="485"/>
-      <c r="AL2" s="485"/>
-    </row>
-    <row r="3" spans="2:38" x14ac:dyDescent="0.3">
+      <c r="AG2" s="460"/>
+      <c r="AH2" s="458"/>
+      <c r="AI2" s="458"/>
+      <c r="AJ2" s="458"/>
+      <c r="AK2" s="452"/>
+      <c r="AL2" s="452"/>
+    </row>
+    <row r="3" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="14">
         <v>0.37</v>
       </c>
@@ -9613,7 +9612,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="2:38" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="28">
         <v>0.44</v>
       </c>
@@ -9730,7 +9729,7 @@
         <v>4.4862982062414796</v>
       </c>
     </row>
-    <row r="5" spans="2:38" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="28">
         <v>0.52</v>
       </c>
@@ -9847,7 +9846,7 @@
         <v>4.6747701009495621</v>
       </c>
     </row>
-    <row r="6" spans="2:38" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="28">
         <v>0.61</v>
       </c>
@@ -9964,7 +9963,7 @@
         <v>4.5354006526071435</v>
       </c>
     </row>
-    <row r="7" spans="2:38" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="28">
         <v>0.72</v>
       </c>
@@ -10081,7 +10080,7 @@
         <v>4.7942747635056886</v>
       </c>
     </row>
-    <row r="8" spans="2:38" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="28">
         <v>0.85</v>
       </c>
@@ -10198,7 +10197,7 @@
         <v>5.2577078294667103</v>
       </c>
     </row>
-    <row r="9" spans="2:38" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="28">
         <v>1.01</v>
       </c>
@@ -10315,7 +10314,7 @@
         <v>5.6995853735103816</v>
       </c>
     </row>
-    <row r="10" spans="2:38" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="28">
         <v>1.19</v>
       </c>
@@ -10432,7 +10431,7 @@
         <v>5.7620190171509806</v>
       </c>
     </row>
-    <row r="11" spans="2:38" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="28">
         <v>1.4</v>
       </c>
@@ -10549,7 +10548,7 @@
         <v>5.4028394533867061</v>
       </c>
     </row>
-    <row r="12" spans="2:38" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="28">
         <v>1.65</v>
       </c>
@@ -10666,7 +10665,7 @@
         <v>4.0131920254947007</v>
       </c>
     </row>
-    <row r="13" spans="2:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="42">
         <v>1.95</v>
       </c>
@@ -10783,7 +10782,7 @@
         <v>4.1655882664049999</v>
       </c>
     </row>
-    <row r="14" spans="2:38" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="28">
         <v>2.2999999999999998</v>
       </c>
@@ -10900,7 +10899,7 @@
         <v>4.4084484937594492</v>
       </c>
     </row>
-    <row r="15" spans="2:38" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="28">
         <v>2.72</v>
       </c>
@@ -11017,7 +11016,7 @@
         <v>4.116314199395771</v>
       </c>
     </row>
-    <row r="16" spans="2:38" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:38" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="28">
         <v>3.2</v>
       </c>
@@ -11090,26 +11089,26 @@
       <c r="Y16" s="41">
         <v>1.1583636475738333</v>
       </c>
-      <c r="AG16" s="476" t="s">
+      <c r="AG16" s="458" t="s">
         <v>56</v>
       </c>
-      <c r="AH16" s="476" t="s">
+      <c r="AH16" s="458" t="s">
         <v>57</v>
       </c>
-      <c r="AI16" s="476" t="s">
+      <c r="AI16" s="458" t="s">
         <v>52</v>
       </c>
-      <c r="AJ16" s="476" t="s">
+      <c r="AJ16" s="458" t="s">
         <v>56</v>
       </c>
-      <c r="AK16" s="485" t="s">
+      <c r="AK16" s="452" t="s">
         <v>57</v>
       </c>
-      <c r="AL16" s="485" t="s">
+      <c r="AL16" s="452" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="2:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="28">
         <v>3.78</v>
       </c>
@@ -11182,25 +11181,25 @@
       <c r="Y17" s="41">
         <v>1.2284974412725813</v>
       </c>
-      <c r="AB17" s="488" t="s">
+      <c r="AB17" s="455" t="s">
         <v>40</v>
       </c>
-      <c r="AC17" s="490"/>
-      <c r="AD17" s="483" t="s">
+      <c r="AC17" s="457"/>
+      <c r="AD17" s="459" t="s">
         <v>58</v>
       </c>
-      <c r="AE17" s="483"/>
+      <c r="AE17" s="459"/>
       <c r="AF17" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="AG17" s="476"/>
-      <c r="AH17" s="476"/>
-      <c r="AI17" s="476"/>
-      <c r="AJ17" s="476"/>
-      <c r="AK17" s="485"/>
-      <c r="AL17" s="485"/>
-    </row>
-    <row r="18" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="AG17" s="458"/>
+      <c r="AH17" s="458"/>
+      <c r="AI17" s="458"/>
+      <c r="AJ17" s="458"/>
+      <c r="AK17" s="452"/>
+      <c r="AL17" s="452"/>
+    </row>
+    <row r="18" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="28">
         <v>4.46</v>
       </c>
@@ -11308,7 +11307,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" s="28">
         <v>5.27</v>
       </c>
@@ -11425,7 +11424,7 @@
         <v>4.5587550186087658</v>
       </c>
     </row>
-    <row r="20" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="28">
         <v>6.21</v>
       </c>
@@ -11542,7 +11541,7 @@
         <v>3.9878514411911556</v>
       </c>
     </row>
-    <row r="21" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" s="28">
         <v>7.33</v>
       </c>
@@ -11659,7 +11658,7 @@
         <v>4.1099541035384686</v>
       </c>
     </row>
-    <row r="22" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" s="28">
         <v>8.65</v>
       </c>
@@ -11776,7 +11775,7 @@
         <v>4.9294166633087526</v>
       </c>
     </row>
-    <row r="23" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" s="28">
         <v>10.210000000000001</v>
       </c>
@@ -11893,7 +11892,7 @@
         <v>5.1075992693696532</v>
       </c>
     </row>
-    <row r="24" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" s="28">
         <v>12.05</v>
       </c>
@@ -12010,7 +12009,7 @@
         <v>4.0737324532326404</v>
       </c>
     </row>
-    <row r="25" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" s="28">
         <v>14.22</v>
       </c>
@@ -12127,7 +12126,7 @@
         <v>5.3576987503520641</v>
       </c>
     </row>
-    <row r="26" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" s="28">
         <v>16.78</v>
       </c>
@@ -12244,7 +12243,7 @@
         <v>5.1676289024362116</v>
       </c>
     </row>
-    <row r="27" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B27" s="28">
         <v>19.809999999999999</v>
       </c>
@@ -12361,7 +12360,7 @@
         <v>4.2478099958744497</v>
       </c>
     </row>
-    <row r="28" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B28" s="28">
         <v>23.37</v>
       </c>
@@ -12478,7 +12477,7 @@
         <v>3.8645229263535508</v>
       </c>
     </row>
-    <row r="29" spans="2:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="28">
         <v>27.58</v>
       </c>
@@ -12595,7 +12594,7 @@
         <v>4.1952896284577506</v>
       </c>
     </row>
-    <row r="30" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" s="28">
         <v>32.549999999999997</v>
       </c>
@@ -12669,7 +12668,7 @@
         <v>5.6565602071644365</v>
       </c>
     </row>
-    <row r="31" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B31" s="28">
         <v>38.409999999999997</v>
       </c>
@@ -12744,7 +12743,7 @@
       </c>
       <c r="AG31" s="83"/>
     </row>
-    <row r="32" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B32" s="28">
         <v>45.32</v>
       </c>
@@ -12817,14 +12816,14 @@
       <c r="Y32" s="41">
         <v>6.9971946482520506</v>
       </c>
-      <c r="AA32" s="486" t="s">
+      <c r="AA32" s="453" t="s">
         <v>25</v>
       </c>
-      <c r="AB32" s="486"/>
-      <c r="AC32" s="487" t="s">
+      <c r="AB32" s="453"/>
+      <c r="AC32" s="454" t="s">
         <v>40</v>
       </c>
-      <c r="AD32" s="487"/>
+      <c r="AD32" s="454"/>
       <c r="AI32" s="240" t="s">
         <v>76</v>
       </c>
@@ -12841,7 +12840,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="2:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="28">
         <v>53.48</v>
       </c>
@@ -12946,7 +12945,7 @@
         <v>-3.1232600058148624E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B34" s="14">
         <v>63.11</v>
       </c>
@@ -13055,7 +13054,7 @@
         <v>-8.6593108308677155E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B35" s="28">
         <v>74.48</v>
       </c>
@@ -13164,7 +13163,7 @@
         <v>6.5999564974747599E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B36" s="28">
         <v>87.89</v>
       </c>
@@ -13273,7 +13272,7 @@
         <v>0.11179122774730278</v>
       </c>
     </row>
-    <row r="37" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B37" s="28">
         <v>103.72</v>
       </c>
@@ -13382,7 +13381,7 @@
         <v>-0.17582642709759408</v>
       </c>
     </row>
-    <row r="38" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B38" s="28">
         <v>122.39</v>
       </c>
@@ -13491,7 +13490,7 @@
         <v>-0.11171399488573321</v>
       </c>
     </row>
-    <row r="39" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="28">
         <v>144.43</v>
       </c>
@@ -13600,7 +13599,7 @@
         <v>-7.121946965890269E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B40" s="28">
         <v>170.44</v>
       </c>
@@ -13709,7 +13708,7 @@
         <v>4.7038602982888728E-2</v>
       </c>
     </row>
-    <row r="41" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B41" s="28">
         <v>201.13</v>
       </c>
@@ -13818,7 +13817,7 @@
         <v>4.5512412826442646E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B42" s="28">
         <v>237.35</v>
       </c>
@@ -13927,7 +13926,7 @@
         <v>1.1007356080440442E-2</v>
       </c>
     </row>
-    <row r="43" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B43" s="28">
         <v>280.08999999999997</v>
       </c>
@@ -14036,7 +14035,7 @@
         <v>-6.1936551872839252E-2</v>
       </c>
     </row>
-    <row r="44" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B44" s="28">
         <v>330.52</v>
       </c>
@@ -14126,7 +14125,7 @@
         <v>0.58440306710255763</v>
       </c>
     </row>
-    <row r="45" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B45" s="28">
         <v>390.04</v>
       </c>
@@ -14208,7 +14207,7 @@
         <v>0.89478045810468942</v>
       </c>
     </row>
-    <row r="46" spans="2:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="42">
         <v>460.27</v>
       </c>
@@ -14282,7 +14281,7 @@
         <v>0.86202910167087976</v>
       </c>
     </row>
-    <row r="47" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>24</v>
       </c>
@@ -14356,49 +14355,49 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="2:40" x14ac:dyDescent="0.3">
-      <c r="AA51" s="483" t="s">
+    <row r="51" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="AA51" s="459" t="s">
         <v>104</v>
       </c>
-      <c r="AB51" s="483"/>
-      <c r="AC51" s="483"/>
-      <c r="AD51" s="483"/>
-      <c r="AE51" s="483"/>
-      <c r="AF51" s="483"/>
-      <c r="AG51" s="483"/>
-      <c r="AH51" s="483"/>
-      <c r="AI51" s="483"/>
-      <c r="AJ51" s="483"/>
-      <c r="AK51" s="483"/>
-      <c r="AL51" s="483"/>
-      <c r="AM51" s="483"/>
-      <c r="AN51" s="483"/>
-    </row>
-    <row r="52" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="AB51" s="459"/>
+      <c r="AC51" s="459"/>
+      <c r="AD51" s="459"/>
+      <c r="AE51" s="459"/>
+      <c r="AF51" s="459"/>
+      <c r="AG51" s="459"/>
+      <c r="AH51" s="459"/>
+      <c r="AI51" s="459"/>
+      <c r="AJ51" s="459"/>
+      <c r="AK51" s="459"/>
+      <c r="AL51" s="459"/>
+      <c r="AM51" s="459"/>
+      <c r="AN51" s="459"/>
+    </row>
+    <row r="52" spans="2:40" x14ac:dyDescent="0.2">
       <c r="AA52" s="56"/>
-      <c r="AB52" s="484" t="s">
+      <c r="AB52" s="470" t="s">
         <v>72</v>
       </c>
-      <c r="AC52" s="484"/>
-      <c r="AD52" s="484"/>
-      <c r="AE52" s="484" t="s">
+      <c r="AC52" s="470"/>
+      <c r="AD52" s="470"/>
+      <c r="AE52" s="470" t="s">
         <v>73</v>
       </c>
-      <c r="AF52" s="484"/>
-      <c r="AG52" s="484"/>
-      <c r="AH52" s="484" t="s">
+      <c r="AF52" s="470"/>
+      <c r="AG52" s="470"/>
+      <c r="AH52" s="470" t="s">
         <v>74</v>
       </c>
-      <c r="AI52" s="484"/>
-      <c r="AJ52" s="484"/>
-      <c r="AK52" s="484" t="s">
+      <c r="AI52" s="470"/>
+      <c r="AJ52" s="470"/>
+      <c r="AK52" s="470" t="s">
         <v>75</v>
       </c>
-      <c r="AL52" s="484"/>
-      <c r="AM52" s="484"/>
+      <c r="AL52" s="470"/>
+      <c r="AM52" s="470"/>
       <c r="AN52" s="56"/>
     </row>
-    <row r="53" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:40" ht="15" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>94</v>
       </c>
@@ -14445,7 +14444,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="2:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AA54" s="228" t="s">
         <v>79</v>
       </c>
@@ -14489,35 +14488,35 @@
         <v>0.22851828638601948</v>
       </c>
     </row>
-    <row r="55" spans="2:40" x14ac:dyDescent="0.3">
-      <c r="B55" s="480" t="s">
+    <row r="55" spans="2:40" ht="15" x14ac:dyDescent="0.25">
+      <c r="B55" s="467" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="481"/>
-      <c r="D55" s="481"/>
-      <c r="E55" s="481"/>
-      <c r="F55" s="482"/>
-      <c r="G55" s="480" t="s">
+      <c r="C55" s="468"/>
+      <c r="D55" s="468"/>
+      <c r="E55" s="468"/>
+      <c r="F55" s="469"/>
+      <c r="G55" s="467" t="s">
         <v>2</v>
       </c>
-      <c r="H55" s="481"/>
-      <c r="I55" s="481"/>
-      <c r="J55" s="481"/>
-      <c r="K55" s="482"/>
-      <c r="L55" s="480" t="s">
+      <c r="H55" s="468"/>
+      <c r="I55" s="468"/>
+      <c r="J55" s="468"/>
+      <c r="K55" s="469"/>
+      <c r="L55" s="467" t="s">
         <v>3</v>
       </c>
-      <c r="M55" s="481"/>
-      <c r="N55" s="481"/>
-      <c r="O55" s="481"/>
-      <c r="P55" s="482"/>
-      <c r="Q55" s="480" t="s">
+      <c r="M55" s="468"/>
+      <c r="N55" s="468"/>
+      <c r="O55" s="468"/>
+      <c r="P55" s="469"/>
+      <c r="Q55" s="467" t="s">
         <v>4</v>
       </c>
-      <c r="R55" s="481"/>
-      <c r="S55" s="481"/>
-      <c r="T55" s="481"/>
-      <c r="U55" s="482"/>
+      <c r="R55" s="468"/>
+      <c r="S55" s="468"/>
+      <c r="T55" s="468"/>
+      <c r="U55" s="469"/>
       <c r="AA55" s="228" t="s">
         <v>80</v>
       </c>
@@ -14561,7 +14560,7 @@
         <v>0.22851828638601948</v>
       </c>
     </row>
-    <row r="56" spans="2:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="97" t="s">
         <v>65</v>
       </c>
@@ -14665,7 +14664,7 @@
         <v>-0.3027637470411495</v>
       </c>
     </row>
-    <row r="57" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:40" ht="15" x14ac:dyDescent="0.25">
       <c r="B57" s="170">
         <v>5</v>
       </c>
@@ -14769,7 +14768,7 @@
         <v>-9.3318329100743891E-2</v>
       </c>
     </row>
-    <row r="58" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:40" ht="15" x14ac:dyDescent="0.25">
       <c r="B58" s="173">
         <v>1</v>
       </c>
@@ -14873,7 +14872,7 @@
         <v>5.0766638815107075E-2</v>
       </c>
     </row>
-    <row r="59" spans="2:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="175">
         <v>0.85</v>
       </c>
@@ -14977,7 +14976,7 @@
         <v>5.0766638815107075E-2</v>
       </c>
     </row>
-    <row r="60" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:40" ht="15" x14ac:dyDescent="0.25">
       <c r="B60" s="170">
         <v>0.3</v>
       </c>
@@ -15081,7 +15080,7 @@
         <v>-3.8520880931257544E-2</v>
       </c>
     </row>
-    <row r="61" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:40" ht="15" x14ac:dyDescent="0.25">
       <c r="B61" s="173">
         <v>0.25</v>
       </c>
@@ -15185,7 +15184,7 @@
         <v>-3.8520880931257544E-2</v>
       </c>
     </row>
-    <row r="62" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:40" ht="15" x14ac:dyDescent="0.25">
       <c r="B62" s="173">
         <v>0.125</v>
       </c>
@@ -15289,7 +15288,7 @@
         <v>-6.340384840026668E-2</v>
       </c>
     </row>
-    <row r="63" spans="2:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="175">
         <v>6.3E-2</v>
       </c>
@@ -15393,7 +15392,7 @@
         <v>-6.340384840026668E-2</v>
       </c>
     </row>
-    <row r="64" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:40" ht="15" x14ac:dyDescent="0.25">
       <c r="B64" s="170">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -15497,7 +15496,7 @@
         <v>-3.2730377491297959E-2</v>
       </c>
     </row>
-    <row r="65" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B65" s="173">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -15559,7 +15558,7 @@
         <v>0.76774197914340903</v>
       </c>
     </row>
-    <row r="66" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B66" s="175">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -15621,7 +15620,7 @@
         <v>0.25681629007044648</v>
       </c>
     </row>
-    <row r="67" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B67" s="153" t="s">
         <v>70</v>
       </c>
@@ -15683,7 +15682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="148" t="s">
         <v>24</v>
       </c>
@@ -15726,24 +15725,24 @@
       <c r="T68" s="151"/>
       <c r="U68" s="152"/>
     </row>
-    <row r="69" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="70" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B70" s="452" t="s">
+    <row r="69" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B70" s="461" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="453"/>
-      <c r="D70" s="453"/>
-      <c r="E70" s="453"/>
-      <c r="F70" s="454"/>
-      <c r="G70" s="452" t="s">
+      <c r="C70" s="462"/>
+      <c r="D70" s="462"/>
+      <c r="E70" s="462"/>
+      <c r="F70" s="463"/>
+      <c r="G70" s="461" t="s">
         <v>6</v>
       </c>
-      <c r="H70" s="453"/>
-      <c r="I70" s="453"/>
-      <c r="J70" s="453"/>
-      <c r="K70" s="454"/>
-    </row>
-    <row r="71" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H70" s="462"/>
+      <c r="I70" s="462"/>
+      <c r="J70" s="462"/>
+      <c r="K70" s="463"/>
+    </row>
+    <row r="71" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B71" s="155" t="s">
         <v>65</v>
       </c>
@@ -15775,7 +15774,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B72" s="161">
         <v>5</v>
       </c>
@@ -15807,7 +15806,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B73" s="103">
         <v>1</v>
       </c>
@@ -15839,7 +15838,7 @@
         <v>43.638118564681662</v>
       </c>
     </row>
-    <row r="74" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B74" s="164">
         <v>0.85</v>
       </c>
@@ -15871,7 +15870,7 @@
         <v>34.792354193226231</v>
       </c>
     </row>
-    <row r="75" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B75" s="161">
         <v>0.3</v>
       </c>
@@ -15903,7 +15902,7 @@
         <v>6.7326227226191264</v>
       </c>
     </row>
-    <row r="76" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B76" s="103">
         <v>0.25</v>
       </c>
@@ -15935,7 +15934,7 @@
         <v>5.0779560968669699</v>
       </c>
     </row>
-    <row r="77" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B77" s="103">
         <v>0.125</v>
       </c>
@@ -15967,7 +15966,7 @@
         <v>2.0427035938751033</v>
       </c>
     </row>
-    <row r="78" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B78" s="164">
         <v>6.3E-2</v>
       </c>
@@ -15999,7 +15998,7 @@
         <v>0.97190567716775433</v>
       </c>
     </row>
-    <row r="79" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B79" s="161">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -16031,7 +16030,7 @@
         <v>0.8055044899029582</v>
       </c>
     </row>
-    <row r="80" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B80" s="103">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -16063,7 +16062,7 @@
         <v>0.4286260255362464</v>
       </c>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B81" s="103">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -16095,7 +16094,7 @@
         <v>0.10502941660553233</v>
       </c>
     </row>
-    <row r="82" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B82" s="164" t="s">
         <v>70</v>
       </c>
@@ -16127,7 +16126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B83" s="165" t="s">
         <v>24</v>
       </c>
@@ -16147,24 +16146,24 @@
       <c r="J83" s="168"/>
       <c r="K83" s="169"/>
     </row>
-    <row r="84" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B85" s="477" t="s">
+    <row r="84" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B85" s="464" t="s">
         <v>7</v>
       </c>
-      <c r="C85" s="478"/>
-      <c r="D85" s="478"/>
-      <c r="E85" s="478"/>
-      <c r="F85" s="479"/>
-      <c r="G85" s="477" t="s">
+      <c r="C85" s="465"/>
+      <c r="D85" s="465"/>
+      <c r="E85" s="465"/>
+      <c r="F85" s="466"/>
+      <c r="G85" s="464" t="s">
         <v>8</v>
       </c>
-      <c r="H85" s="478"/>
-      <c r="I85" s="478"/>
-      <c r="J85" s="478"/>
-      <c r="K85" s="479"/>
-    </row>
-    <row r="86" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H85" s="465"/>
+      <c r="I85" s="465"/>
+      <c r="J85" s="465"/>
+      <c r="K85" s="466"/>
+    </row>
+    <row r="86" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B86" s="178" t="s">
         <v>65</v>
       </c>
@@ -16196,7 +16195,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B87" s="184">
         <v>5</v>
       </c>
@@ -16228,7 +16227,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B88" s="112">
         <v>1</v>
       </c>
@@ -16260,7 +16259,7 @@
         <v>38.13410958444954</v>
       </c>
     </row>
-    <row r="89" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B89" s="187">
         <v>0.85</v>
       </c>
@@ -16292,7 +16291,7 @@
         <v>30.354753291890873</v>
       </c>
     </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B90" s="184">
         <v>0.3</v>
       </c>
@@ -16324,7 +16323,7 @@
         <v>6.5023063218227861</v>
       </c>
     </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B91" s="112">
         <v>0.25</v>
       </c>
@@ -16356,7 +16355,7 @@
         <v>5.288683424133751</v>
       </c>
     </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B92" s="112">
         <v>0.125</v>
       </c>
@@ -16388,7 +16387,7 @@
         <v>2.7820248706319859</v>
       </c>
     </row>
-    <row r="93" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B93" s="187">
         <v>6.3E-2</v>
       </c>
@@ -16420,7 +16419,7 @@
         <v>1.7243913192573501</v>
       </c>
     </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B94" s="181">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -16452,7 +16451,7 @@
         <v>1.5124520751739823</v>
       </c>
     </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B95" s="112">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -16484,7 +16483,7 @@
         <v>1.0370068609529142</v>
       </c>
     </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B96" s="112">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -16516,7 +16515,7 @@
         <v>0.62627788793004413</v>
       </c>
     </row>
-    <row r="97" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B97" s="114" t="s">
         <v>70</v>
       </c>
@@ -16548,7 +16547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B98" s="116" t="s">
         <v>24</v>
       </c>
@@ -16570,38 +16569,38 @@
       <c r="J98" s="119"/>
       <c r="K98" s="120"/>
     </row>
-    <row r="99" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="100" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B100" s="464" t="s">
+    <row r="99" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B100" s="471" t="s">
         <v>9</v>
       </c>
-      <c r="C100" s="465"/>
-      <c r="D100" s="465"/>
-      <c r="E100" s="465"/>
-      <c r="F100" s="466"/>
-      <c r="G100" s="464" t="s">
+      <c r="C100" s="472"/>
+      <c r="D100" s="472"/>
+      <c r="E100" s="472"/>
+      <c r="F100" s="473"/>
+      <c r="G100" s="471" t="s">
         <v>10</v>
       </c>
-      <c r="H100" s="465"/>
-      <c r="I100" s="465"/>
-      <c r="J100" s="465"/>
-      <c r="K100" s="466"/>
-      <c r="L100" s="467" t="s">
+      <c r="H100" s="472"/>
+      <c r="I100" s="472"/>
+      <c r="J100" s="472"/>
+      <c r="K100" s="473"/>
+      <c r="L100" s="474" t="s">
         <v>11</v>
       </c>
-      <c r="M100" s="468"/>
-      <c r="N100" s="468"/>
-      <c r="O100" s="468"/>
-      <c r="P100" s="469"/>
-      <c r="Q100" s="464" t="s">
+      <c r="M100" s="475"/>
+      <c r="N100" s="475"/>
+      <c r="O100" s="475"/>
+      <c r="P100" s="476"/>
+      <c r="Q100" s="471" t="s">
         <v>12</v>
       </c>
-      <c r="R100" s="465"/>
-      <c r="S100" s="465"/>
-      <c r="T100" s="465"/>
-      <c r="U100" s="466"/>
-    </row>
-    <row r="101" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R100" s="472"/>
+      <c r="S100" s="472"/>
+      <c r="T100" s="472"/>
+      <c r="U100" s="473"/>
+    </row>
+    <row r="101" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B101" s="188" t="s">
         <v>65</v>
       </c>
@@ -16663,7 +16662,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="102" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B102" s="194">
         <v>5</v>
       </c>
@@ -16725,7 +16724,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B103" s="121">
         <v>1</v>
       </c>
@@ -16787,7 +16786,7 @@
         <v>57.614897190092236</v>
       </c>
     </row>
-    <row r="104" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B104" s="197">
         <v>0.85</v>
       </c>
@@ -16849,7 +16848,7 @@
         <v>49.683536269101168</v>
       </c>
     </row>
-    <row r="105" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B105" s="194">
         <v>0.3</v>
       </c>
@@ -16911,7 +16910,7 @@
         <v>14.041921923228983</v>
       </c>
     </row>
-    <row r="106" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B106" s="121">
         <v>0.25</v>
       </c>
@@ -16973,7 +16972,7 @@
         <v>11.205899101569443</v>
       </c>
     </row>
-    <row r="107" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B107" s="121">
         <v>0.125</v>
       </c>
@@ -17035,7 +17034,7 @@
         <v>5.4972198343870105</v>
       </c>
     </row>
-    <row r="108" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B108" s="197">
         <v>6.3E-2</v>
       </c>
@@ -17097,7 +17096,7 @@
         <v>3.0282586696554006</v>
       </c>
     </row>
-    <row r="109" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B109" s="191">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -17159,7 +17158,7 @@
         <v>2.4950762233272883</v>
       </c>
     </row>
-    <row r="110" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B110" s="121">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -17221,7 +17220,7 @@
         <v>1.3938912525435114</v>
       </c>
     </row>
-    <row r="111" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B111" s="121">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -17283,7 +17282,7 @@
         <v>0.73049622238424661</v>
       </c>
     </row>
-    <row r="112" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B112" s="123" t="s">
         <v>70</v>
       </c>
@@ -17345,7 +17344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B113" s="125" t="s">
         <v>24</v>
       </c>
@@ -17385,38 +17384,38 @@
       <c r="T113" s="128"/>
       <c r="U113" s="129"/>
     </row>
-    <row r="114" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="115" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B115" s="470" t="s">
+    <row r="114" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B115" s="477" t="s">
         <v>13</v>
       </c>
-      <c r="C115" s="471"/>
-      <c r="D115" s="471"/>
-      <c r="E115" s="471"/>
-      <c r="F115" s="472"/>
-      <c r="G115" s="470" t="s">
+      <c r="C115" s="478"/>
+      <c r="D115" s="478"/>
+      <c r="E115" s="478"/>
+      <c r="F115" s="479"/>
+      <c r="G115" s="477" t="s">
         <v>14</v>
       </c>
-      <c r="H115" s="471"/>
-      <c r="I115" s="471"/>
-      <c r="J115" s="471"/>
-      <c r="K115" s="472"/>
-      <c r="L115" s="473" t="s">
+      <c r="H115" s="478"/>
+      <c r="I115" s="478"/>
+      <c r="J115" s="478"/>
+      <c r="K115" s="479"/>
+      <c r="L115" s="480" t="s">
         <v>15</v>
       </c>
-      <c r="M115" s="474"/>
-      <c r="N115" s="474"/>
-      <c r="O115" s="474"/>
-      <c r="P115" s="475"/>
-      <c r="Q115" s="470" t="s">
+      <c r="M115" s="481"/>
+      <c r="N115" s="481"/>
+      <c r="O115" s="481"/>
+      <c r="P115" s="482"/>
+      <c r="Q115" s="477" t="s">
         <v>16</v>
       </c>
-      <c r="R115" s="471"/>
-      <c r="S115" s="471"/>
-      <c r="T115" s="471"/>
-      <c r="U115" s="472"/>
-    </row>
-    <row r="116" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R115" s="478"/>
+      <c r="S115" s="478"/>
+      <c r="T115" s="478"/>
+      <c r="U115" s="479"/>
+    </row>
+    <row r="116" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B116" s="198" t="s">
         <v>65</v>
       </c>
@@ -17478,7 +17477,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="117" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B117" s="204">
         <v>5</v>
       </c>
@@ -17540,7 +17539,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="118" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B118" s="130">
         <v>1</v>
       </c>
@@ -17602,7 +17601,7 @@
         <v>39.693418059151178</v>
       </c>
     </row>
-    <row r="119" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B119" s="207">
         <v>0.85</v>
       </c>
@@ -17664,7 +17663,7 @@
         <v>32.956146544284934</v>
       </c>
     </row>
-    <row r="120" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B120" s="204">
         <v>0.3</v>
       </c>
@@ -17726,7 +17725,7 @@
         <v>7.1524280222797501</v>
       </c>
     </row>
-    <row r="121" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B121" s="130">
         <v>0.25</v>
       </c>
@@ -17788,7 +17787,7 @@
         <v>5.7412724562642126</v>
       </c>
     </row>
-    <row r="122" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B122" s="130">
         <v>0.125</v>
       </c>
@@ -17850,7 +17849,7 @@
         <v>2.6459559111947897</v>
       </c>
     </row>
-    <row r="123" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B123" s="207">
         <v>6.3E-2</v>
       </c>
@@ -17912,7 +17911,7 @@
         <v>1.5172197379775554</v>
       </c>
     </row>
-    <row r="124" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B124" s="201">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -17974,7 +17973,7 @@
         <v>1.3223503569467283</v>
       </c>
     </row>
-    <row r="125" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B125" s="130">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -18036,7 +18035,7 @@
         <v>0.92413901310111157</v>
       </c>
     </row>
-    <row r="126" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B126" s="130">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -18098,7 +18097,7 @@
         <v>0.5136894955675757</v>
       </c>
     </row>
-    <row r="127" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B127" s="132" t="s">
         <v>70</v>
       </c>
@@ -18160,7 +18159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B128" s="134" t="s">
         <v>24</v>
       </c>
@@ -18200,38 +18199,38 @@
       <c r="T128" s="137"/>
       <c r="U128" s="138"/>
     </row>
-    <row r="129" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="130" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B130" s="452" t="s">
+    <row r="129" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B130" s="461" t="s">
         <v>17</v>
       </c>
-      <c r="C130" s="453"/>
-      <c r="D130" s="453"/>
-      <c r="E130" s="453"/>
-      <c r="F130" s="454"/>
-      <c r="G130" s="452" t="s">
+      <c r="C130" s="462"/>
+      <c r="D130" s="462"/>
+      <c r="E130" s="462"/>
+      <c r="F130" s="463"/>
+      <c r="G130" s="461" t="s">
         <v>18</v>
       </c>
-      <c r="H130" s="453"/>
-      <c r="I130" s="453"/>
-      <c r="J130" s="453"/>
-      <c r="K130" s="454"/>
-      <c r="L130" s="455" t="s">
+      <c r="H130" s="462"/>
+      <c r="I130" s="462"/>
+      <c r="J130" s="462"/>
+      <c r="K130" s="463"/>
+      <c r="L130" s="483" t="s">
         <v>19</v>
       </c>
-      <c r="M130" s="456"/>
-      <c r="N130" s="456"/>
-      <c r="O130" s="456"/>
-      <c r="P130" s="457"/>
-      <c r="Q130" s="452" t="s">
+      <c r="M130" s="484"/>
+      <c r="N130" s="484"/>
+      <c r="O130" s="484"/>
+      <c r="P130" s="485"/>
+      <c r="Q130" s="461" t="s">
         <v>20</v>
       </c>
-      <c r="R130" s="453"/>
-      <c r="S130" s="453"/>
-      <c r="T130" s="453"/>
-      <c r="U130" s="454"/>
-    </row>
-    <row r="131" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R130" s="462"/>
+      <c r="S130" s="462"/>
+      <c r="T130" s="462"/>
+      <c r="U130" s="463"/>
+    </row>
+    <row r="131" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B131" s="155" t="s">
         <v>65</v>
       </c>
@@ -18293,7 +18292,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="132" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B132" s="161">
         <v>5</v>
       </c>
@@ -18355,7 +18354,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="133" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B133" s="103">
         <v>1</v>
       </c>
@@ -18417,7 +18416,7 @@
         <v>48.409962359728418</v>
       </c>
     </row>
-    <row r="134" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B134" s="164">
         <v>0.85</v>
       </c>
@@ -18479,7 +18478,7 @@
         <v>39.877581172828641</v>
       </c>
     </row>
-    <row r="135" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B135" s="161">
         <v>0.3</v>
       </c>
@@ -18541,7 +18540,7 @@
         <v>9.2318335854410662</v>
       </c>
     </row>
-    <row r="136" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B136" s="103">
         <v>0.25</v>
       </c>
@@ -18603,7 +18602,7 @@
         <v>7.8557943738933602</v>
       </c>
     </row>
-    <row r="137" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B137" s="103">
         <v>0.125</v>
       </c>
@@ -18665,7 +18664,7 @@
         <v>4.9946646967085258</v>
       </c>
     </row>
-    <row r="138" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B138" s="164">
         <v>6.3E-2</v>
       </c>
@@ -18727,7 +18726,7 @@
         <v>2.9936328138741288</v>
       </c>
     </row>
-    <row r="139" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B139" s="158">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -18789,7 +18788,7 @@
         <v>2.3639497660674635</v>
       </c>
     </row>
-    <row r="140" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B140" s="103">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -18851,7 +18850,7 @@
         <v>1.244122371923396</v>
       </c>
     </row>
-    <row r="141" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B141" s="103">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -18913,7 +18912,7 @@
         <v>0.28669926478346497</v>
       </c>
     </row>
-    <row r="142" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B142" s="105" t="s">
         <v>70</v>
       </c>
@@ -18975,7 +18974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="107" t="s">
         <v>24</v>
       </c>
@@ -19015,31 +19014,31 @@
       <c r="T143" s="110"/>
       <c r="U143" s="111"/>
     </row>
-    <row r="144" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B145" s="458" t="s">
+    <row r="144" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="145" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B145" s="486" t="s">
         <v>21</v>
       </c>
-      <c r="C145" s="459"/>
-      <c r="D145" s="459"/>
-      <c r="E145" s="459"/>
-      <c r="F145" s="460"/>
-      <c r="G145" s="458" t="s">
+      <c r="C145" s="487"/>
+      <c r="D145" s="487"/>
+      <c r="E145" s="487"/>
+      <c r="F145" s="488"/>
+      <c r="G145" s="486" t="s">
         <v>22</v>
       </c>
-      <c r="H145" s="459"/>
-      <c r="I145" s="459"/>
-      <c r="J145" s="459"/>
-      <c r="K145" s="460"/>
-      <c r="L145" s="461" t="s">
+      <c r="H145" s="487"/>
+      <c r="I145" s="487"/>
+      <c r="J145" s="487"/>
+      <c r="K145" s="488"/>
+      <c r="L145" s="489" t="s">
         <v>23</v>
       </c>
-      <c r="M145" s="462"/>
-      <c r="N145" s="462"/>
-      <c r="O145" s="462"/>
-      <c r="P145" s="463"/>
-    </row>
-    <row r="146" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M145" s="490"/>
+      <c r="N145" s="490"/>
+      <c r="O145" s="490"/>
+      <c r="P145" s="491"/>
+    </row>
+    <row r="146" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B146" s="208" t="s">
         <v>65</v>
       </c>
@@ -19086,7 +19085,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B147" s="214">
         <v>5</v>
       </c>
@@ -19133,7 +19132,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B148" s="139">
         <v>1</v>
       </c>
@@ -19180,7 +19179,7 @@
         <v>49.636163364076339</v>
       </c>
     </row>
-    <row r="149" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B149" s="217">
         <v>0.85</v>
       </c>
@@ -19227,7 +19226,7 @@
         <v>39.957252762304812</v>
       </c>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B150" s="214">
         <v>0.3</v>
       </c>
@@ -19274,7 +19273,7 @@
         <v>7.0761231850972592</v>
       </c>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B151" s="139">
         <v>0.25</v>
       </c>
@@ -19321,7 +19320,7 @@
         <v>5.7083827960916835</v>
       </c>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B152" s="139">
         <v>0.125</v>
       </c>
@@ -19368,7 +19367,7 @@
         <v>2.9988699662131353</v>
       </c>
     </row>
-    <row r="153" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B153" s="217">
         <v>6.3E-2</v>
       </c>
@@ -19415,7 +19414,7 @@
         <v>1.7244429732444502</v>
       </c>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B154" s="211">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -19462,7 +19461,7 @@
         <v>1.4798876814902684</v>
       </c>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B155" s="139">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -19509,7 +19508,7 @@
         <v>0.9605287188384608</v>
       </c>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B156" s="139">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -19556,7 +19555,7 @@
         <v>0.295635101817183</v>
       </c>
     </row>
-    <row r="157" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B157" s="141" t="s">
         <v>70</v>
       </c>
@@ -19603,7 +19602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B158" s="143" t="s">
         <v>24</v>
       </c>
@@ -19636,6 +19635,36 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="G130:K130"/>
+    <mergeCell ref="L130:P130"/>
+    <mergeCell ref="Q130:U130"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="G145:K145"/>
+    <mergeCell ref="L145:P145"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="G100:K100"/>
+    <mergeCell ref="L100:P100"/>
+    <mergeCell ref="Q100:U100"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="G115:K115"/>
+    <mergeCell ref="L115:P115"/>
+    <mergeCell ref="Q115:U115"/>
+    <mergeCell ref="AH16:AH17"/>
+    <mergeCell ref="AI16:AI17"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="G70:K70"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="G85:K85"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="G55:K55"/>
+    <mergeCell ref="L55:P55"/>
+    <mergeCell ref="Q55:U55"/>
+    <mergeCell ref="AA51:AN51"/>
+    <mergeCell ref="AB52:AD52"/>
+    <mergeCell ref="AE52:AG52"/>
+    <mergeCell ref="AH52:AJ52"/>
+    <mergeCell ref="AK52:AM52"/>
     <mergeCell ref="AL1:AL2"/>
     <mergeCell ref="AL16:AL17"/>
     <mergeCell ref="AK16:AK17"/>
@@ -19652,36 +19681,6 @@
     <mergeCell ref="AH1:AH2"/>
     <mergeCell ref="AI1:AI2"/>
     <mergeCell ref="AG16:AG17"/>
-    <mergeCell ref="AH16:AH17"/>
-    <mergeCell ref="AI16:AI17"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="G70:K70"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="G85:K85"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="G55:K55"/>
-    <mergeCell ref="L55:P55"/>
-    <mergeCell ref="Q55:U55"/>
-    <mergeCell ref="AA51:AN51"/>
-    <mergeCell ref="AB52:AD52"/>
-    <mergeCell ref="AE52:AG52"/>
-    <mergeCell ref="AH52:AJ52"/>
-    <mergeCell ref="AK52:AM52"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="G100:K100"/>
-    <mergeCell ref="L100:P100"/>
-    <mergeCell ref="Q100:U100"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="G115:K115"/>
-    <mergeCell ref="L115:P115"/>
-    <mergeCell ref="Q115:U115"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="G130:K130"/>
-    <mergeCell ref="L130:P130"/>
-    <mergeCell ref="Q130:U130"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="G145:K145"/>
-    <mergeCell ref="L145:P145"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19693,48 +19692,48 @@
   <dimension ref="B1:AM158"/>
   <sheetViews>
     <sheetView topLeftCell="X1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC4" sqref="AC4:AC12"/>
+      <selection activeCell="AB48" sqref="AB48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.75" customWidth="1"/>
     <col min="27" max="27" width="18" customWidth="1"/>
-    <col min="28" max="28" width="22.44140625" customWidth="1"/>
+    <col min="28" max="28" width="22.5" customWidth="1"/>
     <col min="29" max="29" width="19" customWidth="1"/>
-    <col min="30" max="30" width="18.6640625" customWidth="1"/>
-    <col min="31" max="31" width="16.77734375" customWidth="1"/>
-    <col min="32" max="32" width="19.109375" customWidth="1"/>
-    <col min="33" max="33" width="20.88671875" customWidth="1"/>
-    <col min="34" max="34" width="17.33203125" customWidth="1"/>
-    <col min="35" max="35" width="20.21875" customWidth="1"/>
-    <col min="36" max="36" width="18.21875" customWidth="1"/>
+    <col min="30" max="30" width="18.625" customWidth="1"/>
+    <col min="31" max="31" width="16.75" customWidth="1"/>
+    <col min="32" max="32" width="19.125" customWidth="1"/>
+    <col min="33" max="33" width="20.875" customWidth="1"/>
+    <col min="34" max="34" width="17.375" customWidth="1"/>
+    <col min="35" max="35" width="20.25" customWidth="1"/>
+    <col min="36" max="36" width="18.25" customWidth="1"/>
     <col min="37" max="37" width="17" customWidth="1"/>
-    <col min="38" max="38" width="14.5546875" customWidth="1"/>
-    <col min="39" max="39" width="14.6640625" customWidth="1"/>
+    <col min="38" max="38" width="14.5" customWidth="1"/>
+    <col min="39" max="39" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="AF1" s="476" t="s">
+    <row r="1" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AF1" s="458" t="s">
         <v>56</v>
       </c>
-      <c r="AG1" s="476" t="s">
+      <c r="AG1" s="458" t="s">
         <v>57</v>
       </c>
-      <c r="AH1" s="476" t="s">
+      <c r="AH1" s="458" t="s">
         <v>52</v>
       </c>
-      <c r="AI1" s="476" t="s">
+      <c r="AI1" s="458" t="s">
         <v>56</v>
       </c>
-      <c r="AJ1" s="476" t="s">
+      <c r="AJ1" s="458" t="s">
         <v>57</v>
       </c>
-      <c r="AK1" s="476" t="s">
+      <c r="AK1" s="458" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -19807,22 +19806,22 @@
       <c r="Y2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AB2" s="488" t="s">
+      <c r="AB2" s="455" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="489"/>
-      <c r="AD2" s="483" t="s">
+      <c r="AC2" s="456"/>
+      <c r="AD2" s="459" t="s">
         <v>58</v>
       </c>
-      <c r="AE2" s="483"/>
-      <c r="AF2" s="476"/>
-      <c r="AG2" s="476"/>
-      <c r="AH2" s="476"/>
-      <c r="AI2" s="476"/>
-      <c r="AJ2" s="476"/>
-      <c r="AK2" s="476"/>
-    </row>
-    <row r="3" spans="2:37" x14ac:dyDescent="0.3">
+      <c r="AE2" s="459"/>
+      <c r="AF2" s="458"/>
+      <c r="AG2" s="458"/>
+      <c r="AH2" s="458"/>
+      <c r="AI2" s="458"/>
+      <c r="AJ2" s="458"/>
+      <c r="AK2" s="458"/>
+    </row>
+    <row r="3" spans="2:37" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="14">
         <v>0.37</v>
       </c>
@@ -19925,7 +19924,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:37" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="28">
         <v>0.44</v>
       </c>
@@ -20035,7 +20034,7 @@
         <v>4.4862982062414751</v>
       </c>
     </row>
-    <row r="5" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:37" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="28">
         <v>0.52</v>
       </c>
@@ -20145,7 +20144,7 @@
         <v>4.6747701009495621</v>
       </c>
     </row>
-    <row r="6" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:37" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="28">
         <v>0.61</v>
       </c>
@@ -20255,7 +20254,7 @@
         <v>4.5354006526071435</v>
       </c>
     </row>
-    <row r="7" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:37" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="28">
         <v>0.72</v>
       </c>
@@ -20365,7 +20364,7 @@
         <v>4.7942747635056886</v>
       </c>
     </row>
-    <row r="8" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:37" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="28">
         <v>0.85</v>
       </c>
@@ -20475,7 +20474,7 @@
         <v>5.2577078294667103</v>
       </c>
     </row>
-    <row r="9" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:37" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="28">
         <v>1.01</v>
       </c>
@@ -20585,7 +20584,7 @@
         <v>5.6995853735103816</v>
       </c>
     </row>
-    <row r="10" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:37" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="28">
         <v>1.19</v>
       </c>
@@ -20695,7 +20694,7 @@
         <v>5.4028394533867061</v>
       </c>
     </row>
-    <row r="11" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:37" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="28">
         <v>1.4</v>
       </c>
@@ -20805,7 +20804,7 @@
         <v>4.0131920254947007</v>
       </c>
     </row>
-    <row r="12" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:37" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="28">
         <v>1.65</v>
       </c>
@@ -20915,7 +20914,7 @@
         <v>4.1655882664049999</v>
       </c>
     </row>
-    <row r="13" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="42">
         <v>1.95</v>
       </c>
@@ -21025,7 +21024,7 @@
         <v>4.4084484937594492</v>
       </c>
     </row>
-    <row r="14" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:37" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="28">
         <v>2.2999999999999998</v>
       </c>
@@ -21135,7 +21134,7 @@
         <v>4.116314199395771</v>
       </c>
     </row>
-    <row r="15" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:37" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="28">
         <v>2.72</v>
       </c>
@@ -21206,26 +21205,26 @@
       <c r="Y15" s="402">
         <v>1.0235026535253984</v>
       </c>
-      <c r="AF15" s="476" t="s">
+      <c r="AF15" s="458" t="s">
         <v>56</v>
       </c>
-      <c r="AG15" s="476" t="s">
+      <c r="AG15" s="458" t="s">
         <v>57</v>
       </c>
-      <c r="AH15" s="476" t="s">
+      <c r="AH15" s="458" t="s">
         <v>52</v>
       </c>
-      <c r="AI15" s="476" t="s">
+      <c r="AI15" s="458" t="s">
         <v>56</v>
       </c>
-      <c r="AJ15" s="476" t="s">
+      <c r="AJ15" s="458" t="s">
         <v>57</v>
       </c>
-      <c r="AK15" s="476" t="s">
+      <c r="AK15" s="458" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:37" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="28">
         <v>3.2</v>
       </c>
@@ -21296,22 +21295,22 @@
       <c r="Y16" s="402">
         <v>1.0708870356330553</v>
       </c>
-      <c r="AB16" s="488" t="s">
+      <c r="AB16" s="455" t="s">
         <v>40</v>
       </c>
-      <c r="AC16" s="490"/>
-      <c r="AD16" s="483" t="s">
+      <c r="AC16" s="457"/>
+      <c r="AD16" s="459" t="s">
         <v>58</v>
       </c>
-      <c r="AE16" s="483"/>
-      <c r="AF16" s="476"/>
-      <c r="AG16" s="476"/>
-      <c r="AH16" s="476"/>
-      <c r="AI16" s="476"/>
-      <c r="AJ16" s="476"/>
-      <c r="AK16" s="476"/>
-    </row>
-    <row r="17" spans="2:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE16" s="459"/>
+      <c r="AF16" s="458"/>
+      <c r="AG16" s="458"/>
+      <c r="AH16" s="458"/>
+      <c r="AI16" s="458"/>
+      <c r="AJ16" s="458"/>
+      <c r="AK16" s="458"/>
+    </row>
+    <row r="17" spans="2:39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="28">
         <v>3.78</v>
       </c>
@@ -21414,7 +21413,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="28">
         <v>4.46</v>
       </c>
@@ -21524,7 +21523,7 @@
         <v>4.5587550186087658</v>
       </c>
     </row>
-    <row r="19" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" s="28">
         <v>5.27</v>
       </c>
@@ -21634,7 +21633,7 @@
         <v>3.9878514411911556</v>
       </c>
     </row>
-    <row r="20" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="28">
         <v>6.21</v>
       </c>
@@ -21744,7 +21743,7 @@
         <v>4.1099541035384686</v>
       </c>
     </row>
-    <row r="21" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" s="28">
         <v>7.33</v>
       </c>
@@ -21854,7 +21853,7 @@
         <v>4.9294166633087526</v>
       </c>
     </row>
-    <row r="22" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" s="28">
         <v>8.65</v>
       </c>
@@ -21964,7 +21963,7 @@
         <v>5.1075992693696532</v>
       </c>
     </row>
-    <row r="23" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" s="28">
         <v>10.210000000000001</v>
       </c>
@@ -22074,7 +22073,7 @@
         <v>4.0737324532326404</v>
       </c>
     </row>
-    <row r="24" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" s="28">
         <v>12.05</v>
       </c>
@@ -22184,7 +22183,7 @@
         <v>5.3576987503520641</v>
       </c>
     </row>
-    <row r="25" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" s="28">
         <v>14.22</v>
       </c>
@@ -22294,7 +22293,7 @@
         <v>5.1676289024362116</v>
       </c>
     </row>
-    <row r="26" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" s="28">
         <v>16.78</v>
       </c>
@@ -22404,7 +22403,7 @@
         <v>4.2478099958744497</v>
       </c>
     </row>
-    <row r="27" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B27" s="28">
         <v>19.809999999999999</v>
       </c>
@@ -22514,7 +22513,7 @@
         <v>3.8645229263535508</v>
       </c>
     </row>
-    <row r="28" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B28" s="28">
         <v>23.37</v>
       </c>
@@ -22624,7 +22623,7 @@
         <v>4.1952896284577506</v>
       </c>
     </row>
-    <row r="29" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B29" s="28">
         <v>27.58</v>
       </c>
@@ -22696,7 +22695,7 @@
         <v>5.8188021228203191</v>
       </c>
     </row>
-    <row r="30" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" s="28">
         <v>32.549999999999997</v>
       </c>
@@ -22769,7 +22768,7 @@
       </c>
       <c r="AG30" s="83"/>
     </row>
-    <row r="31" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B31" s="28">
         <v>38.409999999999997</v>
       </c>
@@ -22840,14 +22839,14 @@
       <c r="Y31" s="402">
         <v>6.6148597422289619</v>
       </c>
-      <c r="AA31" s="486" t="s">
+      <c r="AA31" s="453" t="s">
         <v>25</v>
       </c>
-      <c r="AB31" s="486"/>
-      <c r="AC31" s="487" t="s">
+      <c r="AB31" s="453"/>
+      <c r="AC31" s="454" t="s">
         <v>40</v>
       </c>
-      <c r="AD31" s="487"/>
+      <c r="AD31" s="454"/>
       <c r="AI31" s="240" t="s">
         <v>76</v>
       </c>
@@ -22864,7 +22863,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B32" s="28">
         <v>45.32</v>
       </c>
@@ -22967,7 +22966,7 @@
         <v>6.3534184185566445E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="28">
         <v>53.48</v>
       </c>
@@ -23074,7 +23073,7 @@
         <v>0.2629811061366164</v>
       </c>
     </row>
-    <row r="34" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B34" s="14">
         <v>63.11</v>
       </c>
@@ -23181,7 +23180,7 @@
         <v>0.15471387032590711</v>
       </c>
     </row>
-    <row r="35" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B35" s="28">
         <v>74.48</v>
       </c>
@@ -23288,7 +23287,7 @@
         <v>-0.69693520760422667</v>
       </c>
     </row>
-    <row r="36" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B36" s="28">
         <v>87.89</v>
       </c>
@@ -23395,7 +23394,7 @@
         <v>-0.29223680900475701</v>
       </c>
     </row>
-    <row r="37" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B37" s="28">
         <v>103.72</v>
       </c>
@@ -23502,7 +23501,7 @@
         <v>-0.49982933597448476</v>
       </c>
     </row>
-    <row r="38" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B38" s="28">
         <v>122.39</v>
       </c>
@@ -23609,7 +23608,7 @@
         <v>-0.35734319518113383</v>
       </c>
     </row>
-    <row r="39" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="28">
         <v>144.43</v>
       </c>
@@ -23716,7 +23715,7 @@
         <v>4.394006002168438E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B40" s="28">
         <v>170.44</v>
       </c>
@@ -23823,7 +23822,7 @@
         <v>-0.14455998731665787</v>
       </c>
     </row>
-    <row r="41" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B41" s="28">
         <v>201.13</v>
       </c>
@@ -23930,7 +23929,7 @@
         <v>3.0947982898429927E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B42" s="28">
         <v>237.35</v>
       </c>
@@ -24018,7 +24017,7 @@
         <v>0.5936777493606139</v>
       </c>
     </row>
-    <row r="43" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B43" s="28">
         <v>280.08999999999997</v>
       </c>
@@ -24106,7 +24105,7 @@
         <v>2.1123285725410796</v>
       </c>
     </row>
-    <row r="44" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B44" s="28">
         <v>330.52</v>
       </c>
@@ -24178,7 +24177,7 @@
         <v>2.5208491281273697</v>
       </c>
     </row>
-    <row r="45" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B45" s="28">
         <v>390.04</v>
       </c>
@@ -24250,7 +24249,7 @@
         <v>2.388172858225929</v>
       </c>
     </row>
-    <row r="46" spans="2:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="42">
         <v>460.27</v>
       </c>
@@ -24322,7 +24321,7 @@
         <v>2.1322971948445799</v>
       </c>
     </row>
-    <row r="47" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>24</v>
       </c>
@@ -24397,13 +24396,13 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="55" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B55" s="492" t="s">
         <v>1</v>
       </c>
@@ -24433,7 +24432,7 @@
       <c r="T55" s="493"/>
       <c r="U55" s="494"/>
     </row>
-    <row r="56" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B56" s="97" t="s">
         <v>65</v>
       </c>
@@ -24495,7 +24494,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B57" s="170">
         <v>5</v>
       </c>
@@ -24557,7 +24556,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B58" s="173">
         <v>1</v>
       </c>
@@ -24619,7 +24618,7 @@
         <v>93.215838326871108</v>
       </c>
     </row>
-    <row r="59" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B59" s="175">
         <v>0.85</v>
       </c>
@@ -24681,7 +24680,7 @@
         <v>91.816472799906009</v>
       </c>
     </row>
-    <row r="60" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B60" s="170">
         <v>0.3</v>
       </c>
@@ -24743,7 +24742,7 @@
         <v>70.403007872165432</v>
       </c>
     </row>
-    <row r="61" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B61" s="173">
         <v>0.25</v>
       </c>
@@ -24805,7 +24804,7 @@
         <v>63.588297497356365</v>
       </c>
     </row>
-    <row r="62" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B62" s="173">
         <v>0.125</v>
       </c>
@@ -24867,7 +24866,7 @@
         <v>41.543884384913639</v>
       </c>
     </row>
-    <row r="63" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B63" s="175">
         <v>6.3E-2</v>
       </c>
@@ -24929,7 +24928,7 @@
         <v>23.931382916226056</v>
       </c>
     </row>
-    <row r="64" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B64" s="170">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -24991,7 +24990,7 @@
         <v>20.16214310891786</v>
       </c>
     </row>
-    <row r="65" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B65" s="173">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -25053,7 +25052,7 @@
         <v>10.078721654329684</v>
       </c>
     </row>
-    <row r="66" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B66" s="175">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -25115,7 +25114,7 @@
         <v>0.23616496298906497</v>
       </c>
     </row>
-    <row r="67" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B67" s="153" t="s">
         <v>70</v>
       </c>
@@ -25177,7 +25176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="148" t="s">
         <v>24</v>
       </c>
@@ -25217,24 +25216,24 @@
       <c r="T68" s="151"/>
       <c r="U68" s="152"/>
     </row>
-    <row r="69" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="70" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B70" s="455" t="s">
+    <row r="69" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B70" s="483" t="s">
         <v>95</v>
       </c>
-      <c r="C70" s="456"/>
-      <c r="D70" s="456"/>
-      <c r="E70" s="456"/>
-      <c r="F70" s="457"/>
-      <c r="G70" s="455" t="s">
+      <c r="C70" s="484"/>
+      <c r="D70" s="484"/>
+      <c r="E70" s="484"/>
+      <c r="F70" s="485"/>
+      <c r="G70" s="483" t="s">
         <v>6</v>
       </c>
-      <c r="H70" s="456"/>
-      <c r="I70" s="456"/>
-      <c r="J70" s="456"/>
-      <c r="K70" s="457"/>
-    </row>
-    <row r="71" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H70" s="484"/>
+      <c r="I70" s="484"/>
+      <c r="J70" s="484"/>
+      <c r="K70" s="485"/>
+    </row>
+    <row r="71" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B71" s="155" t="s">
         <v>65</v>
       </c>
@@ -25266,7 +25265,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B72" s="161">
         <v>5</v>
       </c>
@@ -25298,7 +25297,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B73" s="103">
         <v>1</v>
       </c>
@@ -25330,7 +25329,7 @@
         <v>62.622398414271558</v>
       </c>
     </row>
-    <row r="74" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B74" s="164">
         <v>0.85</v>
       </c>
@@ -25362,7 +25361,7 @@
         <v>58.313842087875784</v>
       </c>
     </row>
-    <row r="75" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B75" s="161">
         <v>0.3</v>
       </c>
@@ -25394,7 +25393,7 @@
         <v>36.936901222332338</v>
       </c>
     </row>
-    <row r="76" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B76" s="103">
         <v>0.25</v>
       </c>
@@ -25426,7 +25425,7 @@
         <v>33.714568880079284</v>
       </c>
     </row>
-    <row r="77" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B77" s="103">
         <v>0.125</v>
       </c>
@@ -25458,7 +25457,7 @@
         <v>23.1219028741328</v>
       </c>
     </row>
-    <row r="78" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B78" s="164">
         <v>6.3E-2</v>
       </c>
@@ -25490,7 +25489,7 @@
         <v>14.62371985464155</v>
       </c>
     </row>
-    <row r="79" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B79" s="161">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -25522,7 +25521,7 @@
         <v>12.635612817971577</v>
       </c>
     </row>
-    <row r="80" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B80" s="103">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -25554,7 +25553,7 @@
         <v>7.4364056821935804</v>
       </c>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B81" s="103">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -25586,7 +25585,7 @@
         <v>1.0009910802774868</v>
       </c>
     </row>
-    <row r="82" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B82" s="164" t="s">
         <v>70</v>
       </c>
@@ -25618,7 +25617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B83" s="165" t="s">
         <v>24</v>
       </c>
@@ -25638,8 +25637,8 @@
       <c r="J83" s="168"/>
       <c r="K83" s="169"/>
     </row>
-    <row r="84" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B85" s="495" t="s">
         <v>7</v>
       </c>
@@ -25655,7 +25654,7 @@
       <c r="J85" s="496"/>
       <c r="K85" s="497"/>
     </row>
-    <row r="86" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B86" s="178" t="s">
         <v>65</v>
       </c>
@@ -25687,7 +25686,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B87" s="184">
         <v>5</v>
       </c>
@@ -25719,7 +25718,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B88" s="112">
         <v>1</v>
       </c>
@@ -25751,7 +25750,7 @@
         <v>81.952920210947298</v>
       </c>
     </row>
-    <row r="89" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B89" s="187">
         <v>0.85</v>
       </c>
@@ -25783,7 +25782,7 @@
         <v>77.327828258234291</v>
       </c>
     </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B90" s="184">
         <v>0.3</v>
       </c>
@@ -25815,7 +25814,7 @@
         <v>43.410487271672345</v>
       </c>
     </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B91" s="112">
         <v>0.25</v>
       </c>
@@ -25847,7 +25846,7 @@
         <v>39.51790876218697</v>
       </c>
     </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B92" s="112">
         <v>0.125</v>
       </c>
@@ -25879,7 +25878,7 @@
         <v>26.769895458831087</v>
       </c>
     </row>
-    <row r="93" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B93" s="187">
         <v>6.3E-2</v>
       </c>
@@ -25911,7 +25910,7 @@
         <v>16.913600712827787</v>
       </c>
     </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B94" s="181">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -25943,7 +25942,7 @@
         <v>14.673062776505688</v>
       </c>
     </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B95" s="112">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -25975,7 +25974,7 @@
         <v>8.7114187138017058</v>
       </c>
     </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B96" s="112">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -26007,7 +26006,7 @@
         <v>0.67967301097215227</v>
       </c>
     </row>
-    <row r="97" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B97" s="114" t="s">
         <v>70</v>
       </c>
@@ -26039,7 +26038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B98" s="116" t="s">
         <v>24</v>
       </c>
@@ -26061,38 +26060,38 @@
       <c r="J98" s="119"/>
       <c r="K98" s="120"/>
     </row>
-    <row r="99" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="100" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B100" s="467" t="s">
+    <row r="99" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B100" s="474" t="s">
         <v>9</v>
       </c>
-      <c r="C100" s="468"/>
-      <c r="D100" s="468"/>
-      <c r="E100" s="468"/>
-      <c r="F100" s="469"/>
-      <c r="G100" s="467" t="s">
+      <c r="C100" s="475"/>
+      <c r="D100" s="475"/>
+      <c r="E100" s="475"/>
+      <c r="F100" s="476"/>
+      <c r="G100" s="474" t="s">
         <v>10</v>
       </c>
-      <c r="H100" s="468"/>
-      <c r="I100" s="468"/>
-      <c r="J100" s="468"/>
-      <c r="K100" s="469"/>
-      <c r="L100" s="467" t="s">
+      <c r="H100" s="475"/>
+      <c r="I100" s="475"/>
+      <c r="J100" s="475"/>
+      <c r="K100" s="476"/>
+      <c r="L100" s="474" t="s">
         <v>11</v>
       </c>
-      <c r="M100" s="468"/>
-      <c r="N100" s="468"/>
-      <c r="O100" s="468"/>
-      <c r="P100" s="469"/>
-      <c r="Q100" s="467" t="s">
+      <c r="M100" s="475"/>
+      <c r="N100" s="475"/>
+      <c r="O100" s="475"/>
+      <c r="P100" s="476"/>
+      <c r="Q100" s="474" t="s">
         <v>12</v>
       </c>
-      <c r="R100" s="468"/>
-      <c r="S100" s="468"/>
-      <c r="T100" s="468"/>
-      <c r="U100" s="469"/>
-    </row>
-    <row r="101" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R100" s="475"/>
+      <c r="S100" s="475"/>
+      <c r="T100" s="475"/>
+      <c r="U100" s="476"/>
+    </row>
+    <row r="101" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B101" s="188" t="s">
         <v>65</v>
       </c>
@@ -26154,7 +26153,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="102" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B102" s="194">
         <v>5</v>
       </c>
@@ -26216,7 +26215,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B103" s="121">
         <v>1</v>
       </c>
@@ -26278,7 +26277,7 @@
         <v>69.68717242029139</v>
       </c>
     </row>
-    <row r="104" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B104" s="197">
         <v>0.85</v>
       </c>
@@ -26340,7 +26339,7 @@
         <v>62.622051046488345</v>
       </c>
     </row>
-    <row r="105" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B105" s="194">
         <v>0.3</v>
       </c>
@@ -26402,7 +26401,7 @@
         <v>34.155447981814547</v>
       </c>
     </row>
-    <row r="106" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B106" s="121">
         <v>0.25</v>
       </c>
@@ -26464,7 +26463,7 @@
         <v>31.425273547460051</v>
       </c>
     </row>
-    <row r="107" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B107" s="121">
         <v>0.125</v>
       </c>
@@ -26526,7 +26525,7 @@
         <v>22.252452799076593</v>
       </c>
     </row>
-    <row r="108" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B108" s="197">
         <v>6.3E-2</v>
       </c>
@@ -26588,7 +26587,7 @@
         <v>14.133776191654007</v>
       </c>
     </row>
-    <row r="109" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B109" s="191">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -26650,7 +26649,7 @@
         <v>12.034321519852071</v>
       </c>
     </row>
-    <row r="110" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B110" s="121">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -26712,7 +26711,7 @@
         <v>6.4662026076817085</v>
       </c>
     </row>
-    <row r="111" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B111" s="121">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -26774,7 +26773,7 @@
         <v>1.5017137203632416</v>
       </c>
     </row>
-    <row r="112" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B112" s="123" t="s">
         <v>70</v>
       </c>
@@ -26836,7 +26835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B113" s="125" t="s">
         <v>24</v>
       </c>
@@ -26876,38 +26875,38 @@
       <c r="T113" s="128"/>
       <c r="U113" s="129"/>
     </row>
-    <row r="114" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="115" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B115" s="470" t="s">
+    <row r="114" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B115" s="477" t="s">
         <v>13</v>
       </c>
-      <c r="C115" s="471"/>
-      <c r="D115" s="471"/>
-      <c r="E115" s="471"/>
-      <c r="F115" s="472"/>
-      <c r="G115" s="473" t="s">
+      <c r="C115" s="478"/>
+      <c r="D115" s="478"/>
+      <c r="E115" s="478"/>
+      <c r="F115" s="479"/>
+      <c r="G115" s="480" t="s">
         <v>14</v>
       </c>
-      <c r="H115" s="474"/>
-      <c r="I115" s="474"/>
-      <c r="J115" s="474"/>
-      <c r="K115" s="475"/>
-      <c r="L115" s="473" t="s">
+      <c r="H115" s="481"/>
+      <c r="I115" s="481"/>
+      <c r="J115" s="481"/>
+      <c r="K115" s="482"/>
+      <c r="L115" s="480" t="s">
         <v>15</v>
       </c>
-      <c r="M115" s="474"/>
-      <c r="N115" s="474"/>
-      <c r="O115" s="474"/>
-      <c r="P115" s="475"/>
-      <c r="Q115" s="473" t="s">
+      <c r="M115" s="481"/>
+      <c r="N115" s="481"/>
+      <c r="O115" s="481"/>
+      <c r="P115" s="482"/>
+      <c r="Q115" s="480" t="s">
         <v>16</v>
       </c>
-      <c r="R115" s="474"/>
-      <c r="S115" s="474"/>
-      <c r="T115" s="474"/>
-      <c r="U115" s="475"/>
-    </row>
-    <row r="116" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R115" s="481"/>
+      <c r="S115" s="481"/>
+      <c r="T115" s="481"/>
+      <c r="U115" s="482"/>
+    </row>
+    <row r="116" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B116" s="198" t="s">
         <v>65</v>
       </c>
@@ -26969,7 +26968,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="117" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B117" s="204"/>
       <c r="C117" s="205"/>
       <c r="D117" s="205"/>
@@ -27021,7 +27020,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="118" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B118" s="130"/>
       <c r="C118" s="68"/>
       <c r="D118" s="68"/>
@@ -27073,7 +27072,7 @@
         <v>62.763915547024951</v>
       </c>
     </row>
-    <row r="119" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B119" s="207"/>
       <c r="C119" s="137"/>
       <c r="D119" s="137"/>
@@ -27125,7 +27124,7 @@
         <v>58.108906879902236</v>
       </c>
     </row>
-    <row r="120" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B120" s="204"/>
       <c r="C120" s="205"/>
       <c r="D120" s="205"/>
@@ -27177,7 +27176,7 @@
         <v>31.83789491860874</v>
       </c>
     </row>
-    <row r="121" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B121" s="130"/>
       <c r="C121" s="68"/>
       <c r="D121" s="68"/>
@@ -27229,7 +27228,7 @@
         <v>28.337174318750868</v>
       </c>
     </row>
-    <row r="122" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B122" s="130"/>
       <c r="C122" s="68"/>
       <c r="D122" s="68"/>
@@ -27281,7 +27280,7 @@
         <v>19.184559902768825</v>
       </c>
     </row>
-    <row r="123" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B123" s="207"/>
       <c r="C123" s="137"/>
       <c r="D123" s="137"/>
@@ -27333,7 +27332,7 @@
         <v>12.784836188059955</v>
       </c>
     </row>
-    <row r="124" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B124" s="201"/>
       <c r="C124" s="202"/>
       <c r="D124" s="202"/>
@@ -27385,7 +27384,7 @@
         <v>10.82626569878262</v>
       </c>
     </row>
-    <row r="125" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B125" s="130"/>
       <c r="C125" s="68"/>
       <c r="D125" s="68"/>
@@ -27437,7 +27436,7 @@
         <v>6.5624398116478204</v>
       </c>
     </row>
-    <row r="126" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B126" s="130"/>
       <c r="C126" s="68"/>
       <c r="D126" s="68"/>
@@ -27489,7 +27488,7 @@
         <v>2.2806819464830141</v>
       </c>
     </row>
-    <row r="127" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B127" s="132"/>
       <c r="C127" s="133"/>
       <c r="D127" s="68"/>
@@ -27541,7 +27540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B128" s="134"/>
       <c r="C128" s="135"/>
       <c r="D128" s="136"/>
@@ -27575,38 +27574,38 @@
       <c r="T128" s="137"/>
       <c r="U128" s="138"/>
     </row>
-    <row r="129" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="130" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B130" s="455" t="s">
+    <row r="129" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B130" s="483" t="s">
         <v>17</v>
       </c>
-      <c r="C130" s="456"/>
-      <c r="D130" s="456"/>
-      <c r="E130" s="456"/>
-      <c r="F130" s="457"/>
-      <c r="G130" s="455" t="s">
+      <c r="C130" s="484"/>
+      <c r="D130" s="484"/>
+      <c r="E130" s="484"/>
+      <c r="F130" s="485"/>
+      <c r="G130" s="483" t="s">
         <v>18</v>
       </c>
-      <c r="H130" s="456"/>
-      <c r="I130" s="456"/>
-      <c r="J130" s="456"/>
-      <c r="K130" s="457"/>
-      <c r="L130" s="455" t="s">
+      <c r="H130" s="484"/>
+      <c r="I130" s="484"/>
+      <c r="J130" s="484"/>
+      <c r="K130" s="485"/>
+      <c r="L130" s="483" t="s">
         <v>19</v>
       </c>
-      <c r="M130" s="456"/>
-      <c r="N130" s="456"/>
-      <c r="O130" s="456"/>
-      <c r="P130" s="457"/>
-      <c r="Q130" s="455" t="s">
+      <c r="M130" s="484"/>
+      <c r="N130" s="484"/>
+      <c r="O130" s="484"/>
+      <c r="P130" s="485"/>
+      <c r="Q130" s="483" t="s">
         <v>20</v>
       </c>
-      <c r="R130" s="456"/>
-      <c r="S130" s="456"/>
-      <c r="T130" s="456"/>
-      <c r="U130" s="457"/>
-    </row>
-    <row r="131" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R130" s="484"/>
+      <c r="S130" s="484"/>
+      <c r="T130" s="484"/>
+      <c r="U130" s="485"/>
+    </row>
+    <row r="131" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B131" s="155" t="s">
         <v>65</v>
       </c>
@@ -27668,7 +27667,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="132" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B132" s="161">
         <v>5</v>
       </c>
@@ -27730,7 +27729,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="133" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B133" s="103">
         <v>1</v>
       </c>
@@ -27792,7 +27791,7 @@
         <v>93.219644306574622</v>
       </c>
     </row>
-    <row r="134" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B134" s="164">
         <v>0.85</v>
       </c>
@@ -27854,7 +27853,7 @@
         <v>89.639404338077526</v>
       </c>
     </row>
-    <row r="135" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B135" s="161">
         <v>0.3</v>
       </c>
@@ -27916,7 +27915,7 @@
         <v>57.752364726398945</v>
       </c>
     </row>
-    <row r="136" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B136" s="103">
         <v>0.25</v>
       </c>
@@ -27978,7 +27977,7 @@
         <v>53.000409859120971</v>
       </c>
     </row>
-    <row r="137" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B137" s="103">
         <v>0.125</v>
       </c>
@@ -28040,7 +28039,7 @@
         <v>36.648638222979429</v>
       </c>
     </row>
-    <row r="138" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B138" s="164">
         <v>6.3E-2</v>
       </c>
@@ -28102,7 +28101,7 @@
         <v>23.336253244718037</v>
       </c>
     </row>
-    <row r="139" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B139" s="158">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -28164,7 +28163,7 @@
         <v>20.530727379392928</v>
       </c>
     </row>
-    <row r="140" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B140" s="103">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -28226,7 +28225,7 @@
         <v>12.039410767240199</v>
       </c>
     </row>
-    <row r="141" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B141" s="103">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -28288,7 +28287,7 @@
         <v>1.6322036758737681</v>
       </c>
     </row>
-    <row r="142" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B142" s="105" t="s">
         <v>70</v>
       </c>
@@ -28350,7 +28349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="107" t="s">
         <v>24</v>
       </c>
@@ -28390,31 +28389,31 @@
       <c r="T143" s="110"/>
       <c r="U143" s="111"/>
     </row>
-    <row r="144" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B145" s="461" t="s">
+    <row r="144" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="145" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B145" s="489" t="s">
         <v>21</v>
       </c>
-      <c r="C145" s="462"/>
-      <c r="D145" s="462"/>
-      <c r="E145" s="462"/>
-      <c r="F145" s="463"/>
-      <c r="G145" s="461" t="s">
+      <c r="C145" s="490"/>
+      <c r="D145" s="490"/>
+      <c r="E145" s="490"/>
+      <c r="F145" s="491"/>
+      <c r="G145" s="489" t="s">
         <v>22</v>
       </c>
-      <c r="H145" s="462"/>
-      <c r="I145" s="462"/>
-      <c r="J145" s="462"/>
-      <c r="K145" s="463"/>
-      <c r="L145" s="461" t="s">
+      <c r="H145" s="490"/>
+      <c r="I145" s="490"/>
+      <c r="J145" s="490"/>
+      <c r="K145" s="491"/>
+      <c r="L145" s="489" t="s">
         <v>23</v>
       </c>
-      <c r="M145" s="462"/>
-      <c r="N145" s="462"/>
-      <c r="O145" s="462"/>
-      <c r="P145" s="463"/>
-    </row>
-    <row r="146" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M145" s="490"/>
+      <c r="N145" s="490"/>
+      <c r="O145" s="490"/>
+      <c r="P145" s="491"/>
+    </row>
+    <row r="146" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B146" s="208" t="s">
         <v>65</v>
       </c>
@@ -28461,7 +28460,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B147" s="214">
         <v>5</v>
       </c>
@@ -28508,7 +28507,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B148" s="139">
         <v>1</v>
       </c>
@@ -28555,7 +28554,7 @@
         <v>89.367246568303599</v>
       </c>
     </row>
-    <row r="149" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B149" s="217">
         <v>0.85</v>
       </c>
@@ -28602,7 +28601,7 @@
         <v>84.236952213168905</v>
       </c>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B150" s="214">
         <v>0.3</v>
       </c>
@@ -28649,7 +28648,7 @@
         <v>48.262497247302349</v>
       </c>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B151" s="139">
         <v>0.25</v>
       </c>
@@ -28696,7 +28695,7 @@
         <v>42.709388534096739</v>
       </c>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B152" s="139">
         <v>0.125</v>
       </c>
@@ -28743,7 +28742,7 @@
         <v>26.479483226895681</v>
       </c>
     </row>
-    <row r="153" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B153" s="217">
         <v>6.3E-2</v>
       </c>
@@ -28790,7 +28789,7 @@
         <v>16.325332158848994</v>
       </c>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B154" s="211">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -28837,7 +28836,7 @@
         <v>13.751743375174328</v>
       </c>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B155" s="139">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -28884,7 +28883,7 @@
         <v>7.9196946340747161</v>
       </c>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B156" s="139">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -28931,7 +28930,7 @@
         <v>1.7477794905674102</v>
       </c>
     </row>
-    <row r="157" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B157" s="141" t="s">
         <v>70</v>
       </c>
@@ -28978,7 +28977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B158" s="143" t="s">
         <v>24</v>
       </c>
@@ -29011,24 +29010,17 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="AK1:AK2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF1:AF2"/>
-    <mergeCell ref="AG1:AG2"/>
-    <mergeCell ref="AH1:AH2"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="AJ15:AJ16"/>
-    <mergeCell ref="AK15:AK16"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AD16:AE16"/>
-    <mergeCell ref="AA31:AB31"/>
-    <mergeCell ref="AC31:AD31"/>
-    <mergeCell ref="AI15:AI16"/>
-    <mergeCell ref="AF15:AF16"/>
-    <mergeCell ref="AG15:AG16"/>
-    <mergeCell ref="AH15:AH16"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="G145:K145"/>
+    <mergeCell ref="L145:P145"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="G115:K115"/>
+    <mergeCell ref="L115:P115"/>
+    <mergeCell ref="Q115:U115"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="G130:K130"/>
+    <mergeCell ref="L130:P130"/>
+    <mergeCell ref="Q130:U130"/>
     <mergeCell ref="Q100:U100"/>
     <mergeCell ref="B55:F55"/>
     <mergeCell ref="G55:K55"/>
@@ -29041,17 +29033,24 @@
     <mergeCell ref="B100:F100"/>
     <mergeCell ref="G100:K100"/>
     <mergeCell ref="L100:P100"/>
-    <mergeCell ref="Q115:U115"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="G130:K130"/>
-    <mergeCell ref="L130:P130"/>
-    <mergeCell ref="Q130:U130"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="G145:K145"/>
-    <mergeCell ref="L145:P145"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="G115:K115"/>
-    <mergeCell ref="L115:P115"/>
+    <mergeCell ref="AJ15:AJ16"/>
+    <mergeCell ref="AK15:AK16"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AD16:AE16"/>
+    <mergeCell ref="AA31:AB31"/>
+    <mergeCell ref="AC31:AD31"/>
+    <mergeCell ref="AI15:AI16"/>
+    <mergeCell ref="AF15:AF16"/>
+    <mergeCell ref="AG15:AG16"/>
+    <mergeCell ref="AH15:AH16"/>
+    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF1:AF2"/>
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AJ1:AJ2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -29066,23 +29065,23 @@
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.625" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" customWidth="1"/>
-    <col min="9" max="9" width="18.21875" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" customWidth="1"/>
-    <col min="14" max="14" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="9.25" customWidth="1"/>
+    <col min="5" max="5" width="14.875" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="9" width="18.25" customWidth="1"/>
+    <col min="11" max="11" width="17.625" customWidth="1"/>
+    <col min="12" max="12" width="16.375" customWidth="1"/>
+    <col min="14" max="14" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="483" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="459" t="s">
         <v>96</v>
       </c>
       <c r="B1" s="501"/>
@@ -29097,9 +29096,9 @@
       <c r="K1" s="501"/>
       <c r="L1" s="501"/>
       <c r="M1" s="501"/>
-      <c r="N1" s="483"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N1" s="459"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="239"/>
       <c r="B2" s="498" t="s">
         <v>72</v>
@@ -29123,7 +29122,7 @@
       <c r="M2" s="500"/>
       <c r="N2" s="268"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="240" t="s">
         <v>76</v>
       </c>
@@ -29167,7 +29166,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="241" t="s">
         <v>79</v>
       </c>
@@ -29215,7 +29214,7 @@
         <v>0.22851828638601948</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="241" t="s">
         <v>80</v>
       </c>
@@ -29263,7 +29262,7 @@
         <v>0.22851828638601948</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="242" t="s">
         <v>81</v>
       </c>
@@ -29311,7 +29310,7 @@
         <v>-0.3027637470411495</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="243" t="s">
         <v>82</v>
       </c>
@@ -29359,7 +29358,7 @@
         <v>-9.3318329100743891E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="244" t="s">
         <v>83</v>
       </c>
@@ -29407,7 +29406,7 @@
         <v>5.0766638815107075E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="244" t="s">
         <v>84</v>
       </c>
@@ -29455,7 +29454,7 @@
         <v>5.0766638815107075E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="245" t="s">
         <v>85</v>
       </c>
@@ -29503,7 +29502,7 @@
         <v>-3.8520880931257544E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="245" t="s">
         <v>86</v>
       </c>
@@ -29551,7 +29550,7 @@
         <v>-3.8520880931257544E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="246" t="s">
         <v>87</v>
       </c>
@@ -29599,7 +29598,7 @@
         <v>-6.340384840026668E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="246" t="s">
         <v>88</v>
       </c>
@@ -29647,7 +29646,7 @@
         <v>-6.340384840026668E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="247" t="s">
         <v>89</v>
       </c>
@@ -29695,8 +29694,8 @@
         <v>-3.2730377491297959E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="483" t="s">
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="459" t="s">
         <v>101</v>
       </c>
       <c r="B16" s="501"/>
@@ -29711,9 +29710,9 @@
       <c r="K16" s="501"/>
       <c r="L16" s="501"/>
       <c r="M16" s="501"/>
-      <c r="N16" s="483"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N16" s="459"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="239"/>
       <c r="B17" s="498" t="s">
         <v>72</v>
@@ -29737,7 +29736,7 @@
       <c r="M17" s="500"/>
       <c r="N17" s="268"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="240" t="s">
         <v>76</v>
       </c>
@@ -29781,7 +29780,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="241" t="s">
         <v>79</v>
       </c>
@@ -29829,7 +29828,7 @@
         <v>-0.10058679002726996</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="241" t="s">
         <v>80</v>
       </c>
@@ -29877,7 +29876,7 @@
         <v>-0.10058679002726996</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="242" t="s">
         <v>81</v>
       </c>
@@ -29925,7 +29924,7 @@
         <v>-0.3029856615539851</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="243" t="s">
         <v>82</v>
       </c>
@@ -29973,7 +29972,7 @@
         <v>-0.32001589401318453</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="244" t="s">
         <v>83</v>
       </c>
@@ -30021,7 +30020,7 @@
         <v>0.11743877238132332</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="244" t="s">
         <v>84</v>
       </c>
@@ -30069,7 +30068,7 @@
         <v>0.11743877238132332</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="245" t="s">
         <v>86</v>
       </c>
@@ -30117,7 +30116,7 @@
         <v>-4.5718099286610456E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="246" t="s">
         <v>87</v>
       </c>
@@ -30165,7 +30164,7 @@
         <v>-0.11251612892623995</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="246" t="s">
         <v>88</v>
       </c>
@@ -30213,7 +30212,7 @@
         <v>-0.11251612892623995</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="247" t="s">
         <v>89</v>
       </c>

</xml_diff>